<commit_message>
Swift experiments Plots strategy 1 and 2 and comparison
</commit_message>
<xml_diff>
--- a/Swift_Experiments/strategy_2/analysis/strategy_2_analysis.xlsx
+++ b/Swift_Experiments/strategy_2/analysis/strategy_2_analysis.xlsx
@@ -663,14 +663,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="en-US" sz="1400"/>
               <a:t>Includes: Setup, queuing, bootstrapping, stage in, execution, stage out, shutdown times</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
           <a:p>
             <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -697,7 +692,10 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US" sz="1400"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Queuing time accounts for the majority of the timing and of the variation. </a:t>
+            </a:r>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1010,7 +1008,7 @@
         <c:axId val="-2088925248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="55000.0"/>
+          <c:max val="60000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1297,11 +1295,8 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Includes: Setup, queuing, bootstrapping</a:t>
+              <a:t>Includes: setup, queueing , and bootstrapping times. </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
           <a:p>
             <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -1328,6 +1323,12 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Queuing time accounts for the majority of the timing and of the variation.</a:t>
+            </a:r>
             <a:endParaRPr lang="en-US" sz="1400"/>
           </a:p>
         </c:rich>
@@ -1641,7 +1642,7 @@
         <c:axId val="-2038003120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="55000.0"/>
+          <c:max val="60000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1928,11 +1929,8 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Includes: Setup, queuing, bootstrapping</a:t>
+              <a:t>Includes: stage in, executing , and stage out times. </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
           <a:p>
             <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -1959,6 +1957,12 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>No staging, very little variation mostly due to log/bootstrap overheads.</a:t>
+            </a:r>
             <a:endParaRPr lang="en-US" sz="1400"/>
           </a:p>
         </c:rich>
@@ -2272,7 +2276,7 @@
         <c:axId val="-2030550480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="55000.0"/>
+          <c:max val="60000.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4751,6 +4755,7 @@
       <sheetName val="Tw_stampede_gordon"/>
       <sheetName val="Te_stampede_gordon"/>
       <sheetName val="plots"/>
+      <sheetName val="plots single"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -4803,6 +4808,7 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5506,8 +5512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>